<commit_message>
Pooh Points: final 20260211 -> PD12
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-02-11.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-02-11.xlsx
@@ -434,7 +434,7 @@
     <col width="26" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
     <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="17" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="5" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
@@ -925,14 +925,14 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I6" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J6" t="n">
         <v>3</v>
@@ -947,31 +947,31 @@
         <v>1</v>
       </c>
       <c r="N6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O6" t="n">
         <v>3</v>
       </c>
       <c r="P6" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="Q6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R6" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U6" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="V6" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
@@ -1007,17 +1007,17 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I7" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
         <v>2</v>
@@ -1035,13 +1035,13 @@
         <v>1</v>
       </c>
       <c r="P7" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="Q7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S7" t="n">
         <v>1</v>
@@ -1089,14 +1089,14 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I8" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J8" t="n">
         <v>5</v>
@@ -1117,13 +1117,13 @@
         <v>2</v>
       </c>
       <c r="P8" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="Q8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S8" t="n">
         <v>2</v>
@@ -1499,20 +1499,20 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I13" t="n">
         <v>18</v>
       </c>
       <c r="J13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L13" t="n">
         <v>1</v>
@@ -1521,19 +1521,19 @@
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13" t="n">
         <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="Q13" t="n">
         <v>7</v>
       </c>
       <c r="R13" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="S13" t="n">
         <v>2</v>
@@ -1545,7 +1545,7 @@
         <v>2</v>
       </c>
       <c r="V13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1691,7 +1691,7 @@
         <v>2</v>
       </c>
       <c r="P15" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="Q15" t="n">
         <v>3</v>
@@ -1827,20 +1827,20 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I17" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J17" t="n">
         <v>2</v>
       </c>
       <c r="K17" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L17" t="n">
         <v>0</v>
@@ -1849,25 +1849,25 @@
         <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P17" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="Q17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R17" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="S17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U17" t="n">
         <v>2</v>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -2165,10 +2165,10 @@
         <v>9</v>
       </c>
       <c r="J21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K21" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L21" t="n">
         <v>1</v>
@@ -2177,19 +2177,19 @@
         <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21" t="n">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Q21" t="n">
         <v>3</v>
       </c>
       <c r="R21" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S21" t="n">
         <v>0</v>
@@ -2401,17 +2401,17 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I24" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J24" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K24" t="n">
         <v>0</v>
@@ -2426,16 +2426,16 @@
         <v>2</v>
       </c>
       <c r="O24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P24" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="Q24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S24" t="n">
         <v>0</v>
@@ -3057,47 +3057,47 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I32" t="n">
+        <v>11</v>
+      </c>
+      <c r="J32" t="n">
+        <v>3</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>1</v>
+      </c>
+      <c r="O32" t="n">
+        <v>1</v>
+      </c>
+      <c r="P32" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>4</v>
+      </c>
+      <c r="R32" t="n">
+        <v>11</v>
+      </c>
+      <c r="S32" t="n">
+        <v>1</v>
+      </c>
+      <c r="T32" t="n">
         <v>7</v>
-      </c>
-      <c r="J32" t="n">
-        <v>2</v>
-      </c>
-      <c r="K32" t="n">
-        <v>1</v>
-      </c>
-      <c r="L32" t="n">
-        <v>0</v>
-      </c>
-      <c r="M32" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" t="n">
-        <v>1</v>
-      </c>
-      <c r="O32" t="n">
-        <v>1</v>
-      </c>
-      <c r="P32" t="n">
-        <v>23</v>
-      </c>
-      <c r="Q32" t="n">
-        <v>2</v>
-      </c>
-      <c r="R32" t="n">
-        <v>8</v>
-      </c>
-      <c r="S32" t="n">
-        <v>1</v>
-      </c>
-      <c r="T32" t="n">
-        <v>6</v>
       </c>
       <c r="U32" t="n">
         <v>2</v>
@@ -3139,7 +3139,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H33" t="n">
@@ -3221,23 +3221,23 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I34" t="n">
         <v>3</v>
       </c>
       <c r="J34" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K34" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M34" t="n">
         <v>0</v>
@@ -3249,13 +3249,13 @@
         <v>2</v>
       </c>
       <c r="P34" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="Q34" t="n">
         <v>1</v>
       </c>
       <c r="R34" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S34" t="n">
         <v>0</v>
@@ -3713,11 +3713,11 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I40" t="n">
         <v>12</v>
@@ -3732,16 +3732,16 @@
         <v>0</v>
       </c>
       <c r="M40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N40" t="n">
         <v>0</v>
       </c>
       <c r="O40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P40" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="Q40" t="n">
         <v>3</v>
@@ -3959,20 +3959,20 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I43" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J43" t="n">
         <v>3</v>
       </c>
       <c r="K43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L43" t="n">
         <v>1</v>
@@ -3987,19 +3987,19 @@
         <v>1</v>
       </c>
       <c r="P43" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="Q43" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R43" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="S43" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T43" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="U43" t="n">
         <v>1</v>
@@ -4123,47 +4123,47 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I45" t="n">
+        <v>17</v>
+      </c>
+      <c r="J45" t="n">
+        <v>5</v>
+      </c>
+      <c r="K45" t="n">
+        <v>3</v>
+      </c>
+      <c r="L45" t="n">
+        <v>1</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>2</v>
+      </c>
+      <c r="O45" t="n">
+        <v>1</v>
+      </c>
+      <c r="P45" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>5</v>
+      </c>
+      <c r="R45" t="n">
         <v>14</v>
       </c>
-      <c r="J45" t="n">
+      <c r="S45" t="n">
         <v>4</v>
       </c>
-      <c r="K45" t="n">
-        <v>1</v>
-      </c>
-      <c r="L45" t="n">
-        <v>1</v>
-      </c>
-      <c r="M45" t="n">
-        <v>0</v>
-      </c>
-      <c r="N45" t="n">
-        <v>2</v>
-      </c>
-      <c r="O45" t="n">
-        <v>1</v>
-      </c>
-      <c r="P45" t="n">
-        <v>21</v>
-      </c>
-      <c r="Q45" t="n">
-        <v>4</v>
-      </c>
-      <c r="R45" t="n">
+      <c r="T45" t="n">
         <v>9</v>
-      </c>
-      <c r="S45" t="n">
-        <v>3</v>
-      </c>
-      <c r="T45" t="n">
-        <v>4</v>
       </c>
       <c r="U45" t="n">
         <v>3</v>
@@ -4861,26 +4861,26 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H54" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="I54" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J54" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K54" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L54" t="n">
         <v>1</v>
       </c>
       <c r="M54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N54" t="n">
         <v>1</v>
@@ -4889,13 +4889,13 @@
         <v>1</v>
       </c>
       <c r="P54" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="Q54" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R54" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S54" t="n">
         <v>0</v>
@@ -5025,7 +5025,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H56" t="n">
@@ -5107,7 +5107,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H57" t="n">
@@ -6829,17 +6829,17 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H78" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I78" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J78" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K78" t="n">
         <v>2</v>
@@ -6857,19 +6857,19 @@
         <v>1</v>
       </c>
       <c r="P78" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="Q78" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="R78" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="S78" t="n">
         <v>3</v>
       </c>
       <c r="T78" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U78" t="n">
         <v>0</v>
@@ -6896,68 +6896,68 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Eduardo Klafke</t>
+          <t>Zach Clemence</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>ALA@MISS</t>
+          <t>MIZ@TA&amp;M</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H79" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I79" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J79" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="K79" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O79" t="n">
         <v>4</v>
       </c>
       <c r="P79" t="n">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="Q79" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="R79" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S79" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T79" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -6978,12 +6978,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Zach Clemence</t>
+          <t>T.O. Barrett</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>MIZ</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6993,50 +6993,50 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H80" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I80" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J80" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K80" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L80" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N80" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O80" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P80" t="n">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="Q80" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="R80" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="S80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T80" t="n">
         <v>3</v>
       </c>
       <c r="U80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V80" t="n">
         <v>1</v>
@@ -7060,68 +7060,68 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>T.O. Barrett</t>
+          <t>Eduardo Klafke</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>MIZ</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>MIZ@TA&amp;M</t>
+          <t>ALA@MISS</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H81" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I81" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J81" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="K81" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L81" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N81" t="n">
         <v>2</v>
       </c>
       <c r="O81" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P81" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="Q81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R81" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="S81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T81" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U81" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82">
@@ -7142,68 +7142,68 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Isaiah Brown</t>
+          <t>Bishop Boswell</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>FLA</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>FLA@UGA</t>
+          <t>TENN@MSST</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H82" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I82" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J82" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K82" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M82" t="n">
         <v>0</v>
       </c>
       <c r="N82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O82" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P82" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="Q82" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R82" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S82" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T82" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -7224,56 +7224,56 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>DeWayne Brown II</t>
+          <t>Shawn Phillips Jr.</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>MIZ</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>TENN@MSST</t>
+          <t>MIZ@TA&amp;M</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H83" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I83" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J83" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M83" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N83" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O83" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P83" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="Q83" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R83" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="S83" t="n">
         <v>0</v>
@@ -7285,7 +7285,7 @@
         <v>0</v>
       </c>
       <c r="V83" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84">
@@ -7306,12 +7306,12 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Kanon Catchings</t>
+          <t>Isaiah Brown</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>FLA</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -7325,49 +7325,49 @@
         </is>
       </c>
       <c r="H84" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I84" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J84" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L84" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M84" t="n">
         <v>0</v>
       </c>
       <c r="N84" t="n">
+        <v>0</v>
+      </c>
+      <c r="O84" t="n">
+        <v>3</v>
+      </c>
+      <c r="P84" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q84" t="n">
         <v>4</v>
       </c>
-      <c r="O84" t="n">
-        <v>1</v>
-      </c>
-      <c r="P84" t="n">
-        <v>30</v>
-      </c>
-      <c r="Q84" t="n">
-        <v>3</v>
-      </c>
       <c r="R84" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="S84" t="n">
         <v>3</v>
       </c>
       <c r="T84" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -7388,12 +7388,12 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Shawn Phillips Jr.</t>
+          <t>Ali Dibba</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>MIZ</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -7403,17 +7403,17 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H85" t="n">
         <v>9</v>
       </c>
       <c r="I85" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J85" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K85" t="n">
         <v>1</v>
@@ -7422,34 +7422,34 @@
         <v>0</v>
       </c>
       <c r="M85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N85" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O85" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P85" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="Q85" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R85" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="S85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U85" t="n">
         <v>0</v>
       </c>
       <c r="V85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86">
@@ -7470,62 +7470,62 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Travis Perry</t>
+          <t>DeWayne Brown II</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>ALA@MISS</t>
+          <t>TENN@MSST</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H86" t="n">
         <v>9</v>
       </c>
       <c r="I86" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J86" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M86" t="n">
         <v>0</v>
       </c>
       <c r="N86" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O86" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P86" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="Q86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R86" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S86" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T86" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U86" t="n">
         <v>0</v>
@@ -7552,68 +7552,68 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Achor Achor</t>
+          <t>Kanon Catchings</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>MSST</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>TENN@MSST</t>
+          <t>FLA@UGA</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H87" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I87" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="J87" t="n">
+        <v>8</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0</v>
+      </c>
+      <c r="L87" t="n">
+        <v>2</v>
+      </c>
+      <c r="M87" t="n">
+        <v>0</v>
+      </c>
+      <c r="N87" t="n">
+        <v>4</v>
+      </c>
+      <c r="O87" t="n">
+        <v>1</v>
+      </c>
+      <c r="P87" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q87" t="n">
+        <v>3</v>
+      </c>
+      <c r="R87" t="n">
+        <v>11</v>
+      </c>
+      <c r="S87" t="n">
+        <v>3</v>
+      </c>
+      <c r="T87" t="n">
         <v>6</v>
       </c>
-      <c r="K87" t="n">
-        <v>1</v>
-      </c>
-      <c r="L87" t="n">
-        <v>1</v>
-      </c>
-      <c r="M87" t="n">
-        <v>0</v>
-      </c>
-      <c r="N87" t="n">
-        <v>0</v>
-      </c>
-      <c r="O87" t="n">
-        <v>2</v>
-      </c>
-      <c r="P87" t="n">
-        <v>17</v>
-      </c>
-      <c r="Q87" t="n">
-        <v>1</v>
-      </c>
-      <c r="R87" t="n">
-        <v>5</v>
-      </c>
-      <c r="S87" t="n">
-        <v>1</v>
-      </c>
-      <c r="T87" t="n">
-        <v>3</v>
-      </c>
       <c r="U87" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V87" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88">
@@ -7634,68 +7634,68 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Ali Dibba</t>
+          <t>Travis Perry</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>MIZ@TA&amp;M</t>
+          <t>ALA@MISS</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H88" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I88" t="n">
+        <v>9</v>
+      </c>
+      <c r="J88" t="n">
+        <v>1</v>
+      </c>
+      <c r="K88" t="n">
+        <v>1</v>
+      </c>
+      <c r="L88" t="n">
+        <v>0</v>
+      </c>
+      <c r="M88" t="n">
+        <v>0</v>
+      </c>
+      <c r="N88" t="n">
+        <v>0</v>
+      </c>
+      <c r="O88" t="n">
+        <v>1</v>
+      </c>
+      <c r="P88" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q88" t="n">
+        <v>3</v>
+      </c>
+      <c r="R88" t="n">
         <v>5</v>
       </c>
-      <c r="J88" t="n">
+      <c r="S88" t="n">
+        <v>3</v>
+      </c>
+      <c r="T88" t="n">
         <v>4</v>
       </c>
-      <c r="K88" t="n">
-        <v>1</v>
-      </c>
-      <c r="L88" t="n">
-        <v>0</v>
-      </c>
-      <c r="M88" t="n">
-        <v>0</v>
-      </c>
-      <c r="N88" t="n">
-        <v>1</v>
-      </c>
-      <c r="O88" t="n">
-        <v>1</v>
-      </c>
-      <c r="P88" t="n">
-        <v>11</v>
-      </c>
-      <c r="Q88" t="n">
-        <v>2</v>
-      </c>
-      <c r="R88" t="n">
-        <v>2</v>
-      </c>
-      <c r="S88" t="n">
-        <v>1</v>
-      </c>
-      <c r="T88" t="n">
-        <v>1</v>
-      </c>
       <c r="U88" t="n">
         <v>0</v>
       </c>
       <c r="V88" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -7716,12 +7716,12 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Bishop Boswell</t>
+          <t>Jamarion Davis-Fleming</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>MSST</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -7731,53 +7731,53 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H89" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I89" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J89" t="n">
         <v>4</v>
       </c>
       <c r="K89" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L89" t="n">
         <v>1</v>
       </c>
       <c r="M89" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N89" t="n">
         <v>1</v>
       </c>
       <c r="O89" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P89" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R89" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="S89" t="n">
         <v>0</v>
       </c>
       <c r="T89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U89" t="n">
         <v>0</v>
       </c>
       <c r="V89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -7798,68 +7798,68 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Kareem Stagg</t>
+          <t>Achor Achor</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>MSST</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>FLA@UGA</t>
+          <t>TENN@MSST</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H90" t="n">
         <v>7</v>
       </c>
       <c r="I90" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J90" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K90" t="n">
         <v>1</v>
       </c>
       <c r="L90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M90" t="n">
         <v>0</v>
       </c>
       <c r="N90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P90" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q90" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R90" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="S90" t="n">
         <v>1</v>
       </c>
       <c r="T90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U90" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V90" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -7880,65 +7880,65 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Amari Evans</t>
+          <t>Kareem Stagg</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>TENN@MSST</t>
+          <t>FLA@UGA</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H91" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I91" t="n">
+        <v>9</v>
+      </c>
+      <c r="J91" t="n">
+        <v>2</v>
+      </c>
+      <c r="K91" t="n">
+        <v>1</v>
+      </c>
+      <c r="L91" t="n">
+        <v>0</v>
+      </c>
+      <c r="M91" t="n">
+        <v>0</v>
+      </c>
+      <c r="N91" t="n">
+        <v>1</v>
+      </c>
+      <c r="O91" t="n">
+        <v>1</v>
+      </c>
+      <c r="P91" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q91" t="n">
+        <v>3</v>
+      </c>
+      <c r="R91" t="n">
+        <v>7</v>
+      </c>
+      <c r="S91" t="n">
+        <v>1</v>
+      </c>
+      <c r="T91" t="n">
         <v>4</v>
       </c>
-      <c r="J91" t="n">
-        <v>2</v>
-      </c>
-      <c r="K91" t="n">
-        <v>0</v>
-      </c>
-      <c r="L91" t="n">
-        <v>2</v>
-      </c>
-      <c r="M91" t="n">
-        <v>1</v>
-      </c>
-      <c r="N91" t="n">
-        <v>0</v>
-      </c>
-      <c r="O91" t="n">
-        <v>0</v>
-      </c>
-      <c r="P91" t="n">
-        <v>12</v>
-      </c>
-      <c r="Q91" t="n">
-        <v>1</v>
-      </c>
-      <c r="R91" t="n">
-        <v>3</v>
-      </c>
-      <c r="S91" t="n">
-        <v>1</v>
-      </c>
-      <c r="T91" t="n">
-        <v>1</v>
-      </c>
       <c r="U91" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V91" t="n">
         <v>2</v>
@@ -7977,20 +7977,20 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H92" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J92" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L92" t="n">
         <v>0</v>
@@ -8005,25 +8005,25 @@
         <v>0</v>
       </c>
       <c r="P92" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="Q92" t="n">
         <v>0</v>
       </c>
       <c r="R92" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S92" t="n">
         <v>0</v>
       </c>
       <c r="T92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V92" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
@@ -8044,68 +8044,68 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Zach Day</t>
+          <t>Amari Evans</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>ALA@MISS</t>
+          <t>TENN@MSST</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H93" t="n">
         <v>6</v>
       </c>
       <c r="I93" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J93" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L93" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N93" t="n">
         <v>0</v>
       </c>
       <c r="O93" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P93" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="Q93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R93" t="n">
         <v>3</v>
       </c>
       <c r="S93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T93" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V93" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
@@ -8126,35 +8126,35 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Jamarion Davis-Fleming</t>
+          <t>Zach Day</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>MSST</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>TENN@MSST</t>
+          <t>ALA@MISS</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H94" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I94" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J94" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L94" t="n">
         <v>0</v>
@@ -8163,16 +8163,16 @@
         <v>2</v>
       </c>
       <c r="N94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O94" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P94" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q94" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R94" t="n">
         <v>3</v>
@@ -8181,13 +8181,13 @@
         <v>0</v>
       </c>
       <c r="T94" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U94" t="n">
         <v>0</v>
       </c>
       <c r="V94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -8208,62 +8208,62 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Justin Bailey</t>
+          <t>Jacari Lane</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>FLA@UGA</t>
+          <t>MIZ@TA&amp;M</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H95" t="n">
         <v>5</v>
       </c>
       <c r="I95" t="n">
+        <v>6</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0</v>
+      </c>
+      <c r="K95" t="n">
+        <v>2</v>
+      </c>
+      <c r="L95" t="n">
+        <v>0</v>
+      </c>
+      <c r="M95" t="n">
+        <v>0</v>
+      </c>
+      <c r="N95" t="n">
+        <v>1</v>
+      </c>
+      <c r="O95" t="n">
+        <v>3</v>
+      </c>
+      <c r="P95" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q95" t="n">
+        <v>2</v>
+      </c>
+      <c r="R95" t="n">
         <v>4</v>
       </c>
-      <c r="J95" t="n">
-        <v>3</v>
-      </c>
-      <c r="K95" t="n">
-        <v>1</v>
-      </c>
-      <c r="L95" t="n">
-        <v>1</v>
-      </c>
-      <c r="M95" t="n">
-        <v>0</v>
-      </c>
-      <c r="N95" t="n">
-        <v>0</v>
-      </c>
-      <c r="O95" t="n">
-        <v>1</v>
-      </c>
-      <c r="P95" t="n">
-        <v>21</v>
-      </c>
-      <c r="Q95" t="n">
-        <v>2</v>
-      </c>
-      <c r="R95" t="n">
-        <v>6</v>
-      </c>
       <c r="S95" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T95" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U95" t="n">
         <v>0</v>
@@ -8290,12 +8290,12 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Urban Klavzar</t>
+          <t>Justin Bailey</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>FLA</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -8312,46 +8312,46 @@
         <v>5</v>
       </c>
       <c r="I96" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J96" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K96" t="n">
         <v>1</v>
       </c>
       <c r="L96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M96" t="n">
         <v>0</v>
       </c>
       <c r="N96" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O96" t="n">
         <v>1</v>
       </c>
       <c r="P96" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="Q96" t="n">
         <v>2</v>
       </c>
       <c r="R96" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S96" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T96" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U96" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V96" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -8372,17 +8372,17 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Augusto Cassiá</t>
+          <t>Urban Klavzar</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>FLA</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>ALA@MISS</t>
+          <t>FLA@UGA</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
@@ -8391,49 +8391,49 @@
         </is>
       </c>
       <c r="H97" t="n">
+        <v>5</v>
+      </c>
+      <c r="I97" t="n">
+        <v>8</v>
+      </c>
+      <c r="J97" t="n">
+        <v>1</v>
+      </c>
+      <c r="K97" t="n">
+        <v>1</v>
+      </c>
+      <c r="L97" t="n">
+        <v>0</v>
+      </c>
+      <c r="M97" t="n">
+        <v>0</v>
+      </c>
+      <c r="N97" t="n">
+        <v>2</v>
+      </c>
+      <c r="O97" t="n">
+        <v>1</v>
+      </c>
+      <c r="P97" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q97" t="n">
+        <v>2</v>
+      </c>
+      <c r="R97" t="n">
+        <v>5</v>
+      </c>
+      <c r="S97" t="n">
+        <v>2</v>
+      </c>
+      <c r="T97" t="n">
         <v>4</v>
       </c>
-      <c r="I97" t="n">
-        <v>0</v>
-      </c>
-      <c r="J97" t="n">
-        <v>3</v>
-      </c>
-      <c r="K97" t="n">
-        <v>3</v>
-      </c>
-      <c r="L97" t="n">
-        <v>0</v>
-      </c>
-      <c r="M97" t="n">
-        <v>0</v>
-      </c>
-      <c r="N97" t="n">
-        <v>0</v>
-      </c>
-      <c r="O97" t="n">
-        <v>0</v>
-      </c>
-      <c r="P97" t="n">
-        <v>12</v>
-      </c>
-      <c r="Q97" t="n">
-        <v>0</v>
-      </c>
-      <c r="R97" t="n">
-        <v>2</v>
-      </c>
-      <c r="S97" t="n">
-        <v>0</v>
-      </c>
-      <c r="T97" t="n">
-        <v>0</v>
-      </c>
       <c r="U97" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V97" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98">
@@ -8454,7 +8454,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Corey Chest</t>
+          <t>Augusto Cassiá</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -8476,13 +8476,13 @@
         <v>4</v>
       </c>
       <c r="I98" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K98" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L98" t="n">
         <v>0</v>
@@ -8497,13 +8497,13 @@
         <v>0</v>
       </c>
       <c r="P98" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q98" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S98" t="n">
         <v>0</v>
@@ -8515,7 +8515,7 @@
         <v>0</v>
       </c>
       <c r="V98" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -8536,32 +8536,32 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Jamie Vinson</t>
+          <t>Corey Chest</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>MIZ@TA&amp;M</t>
+          <t>ALA@MISS</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H99" t="n">
         <v>4</v>
       </c>
       <c r="I99" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K99" t="n">
         <v>0</v>
@@ -8570,34 +8570,34 @@
         <v>0</v>
       </c>
       <c r="M99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O99" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P99" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q99" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R99" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U99" t="n">
         <v>0</v>
       </c>
       <c r="V99" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100">
@@ -8618,7 +8618,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Josh Holloway</t>
+          <t>Jamie Vinson</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -8633,17 +8633,17 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H100" t="n">
         <v>4</v>
       </c>
       <c r="I100" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J100" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K100" t="n">
         <v>0</v>
@@ -8652,13 +8652,13 @@
         <v>0</v>
       </c>
       <c r="M100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N100" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O100" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P100" t="n">
         <v>9</v>
@@ -8667,19 +8667,19 @@
         <v>1</v>
       </c>
       <c r="R100" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S100" t="n">
         <v>1</v>
       </c>
       <c r="T100" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U100" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V100" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -8715,7 +8715,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H101" t="n">
@@ -8782,68 +8782,68 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Justin Abson</t>
+          <t>Josh Holloway</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>FLA@UGA</t>
+          <t>MIZ@TA&amp;M</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H102" t="n">
         <v>3</v>
       </c>
       <c r="I102" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J102" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K102" t="n">
         <v>0</v>
       </c>
       <c r="L102" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M102" t="n">
         <v>0</v>
       </c>
       <c r="N102" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O102" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P102" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T102" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U102" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V102" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103">
@@ -8864,17 +8864,17 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Koren Johnson</t>
+          <t>Justin Abson</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>ALA@MISS</t>
+          <t>FLA@UGA</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -8886,40 +8886,40 @@
         <v>3</v>
       </c>
       <c r="I103" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J103" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K103" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M103" t="n">
         <v>0</v>
       </c>
       <c r="N103" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O103" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P103" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="Q103" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R103" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="S103" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T103" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U103" t="n">
         <v>0</v>
@@ -8946,35 +8946,35 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Jacari Lane</t>
+          <t>Koren Johnson</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>MIZ@TA&amp;M</t>
+          <t>ALA@MISS</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H104" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I104" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K104" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L104" t="n">
         <v>0</v>
@@ -8983,25 +8983,25 @@
         <v>0</v>
       </c>
       <c r="N104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O104" t="n">
         <v>3</v>
       </c>
       <c r="P104" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="Q104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R104" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="S104" t="n">
         <v>1</v>
       </c>
       <c r="T104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U104" t="n">
         <v>0</v>
@@ -9125,7 +9125,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H106" t="n">
@@ -9207,7 +9207,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H107" t="n">
@@ -9699,7 +9699,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>18:44 - 2nd Half</t>
+          <t>9:44 - 2nd Half</t>
         </is>
       </c>
       <c r="H113" t="n">
@@ -9781,53 +9781,53 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H114" t="n">
         <v>0</v>
       </c>
       <c r="I114" t="n">
+        <v>6</v>
+      </c>
+      <c r="J114" t="n">
+        <v>0</v>
+      </c>
+      <c r="K114" t="n">
+        <v>1</v>
+      </c>
+      <c r="L114" t="n">
+        <v>2</v>
+      </c>
+      <c r="M114" t="n">
+        <v>0</v>
+      </c>
+      <c r="N114" t="n">
+        <v>3</v>
+      </c>
+      <c r="O114" t="n">
+        <v>1</v>
+      </c>
+      <c r="P114" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q114" t="n">
+        <v>2</v>
+      </c>
+      <c r="R114" t="n">
+        <v>5</v>
+      </c>
+      <c r="S114" t="n">
+        <v>1</v>
+      </c>
+      <c r="T114" t="n">
+        <v>3</v>
+      </c>
+      <c r="U114" t="n">
+        <v>1</v>
+      </c>
+      <c r="V114" t="n">
         <v>4</v>
-      </c>
-      <c r="J114" t="n">
-        <v>0</v>
-      </c>
-      <c r="K114" t="n">
-        <v>1</v>
-      </c>
-      <c r="L114" t="n">
-        <v>1</v>
-      </c>
-      <c r="M114" t="n">
-        <v>0</v>
-      </c>
-      <c r="N114" t="n">
-        <v>3</v>
-      </c>
-      <c r="O114" t="n">
-        <v>1</v>
-      </c>
-      <c r="P114" t="n">
-        <v>19</v>
-      </c>
-      <c r="Q114" t="n">
-        <v>1</v>
-      </c>
-      <c r="R114" t="n">
-        <v>3</v>
-      </c>
-      <c r="S114" t="n">
-        <v>1</v>
-      </c>
-      <c r="T114" t="n">
-        <v>2</v>
-      </c>
-      <c r="U114" t="n">
-        <v>1</v>
-      </c>
-      <c r="V114" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="115">
@@ -10027,7 +10027,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>18:06 - 2nd Half</t>
+          <t>6:43 - 2nd Half</t>
         </is>
       </c>
       <c r="H117" t="n">
@@ -10616,7 +10616,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
@@ -10629,7 +10629,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C3" t="n">
         <v>5</v>
@@ -10642,7 +10642,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C4" t="n">
         <v>5</v>
@@ -10655,7 +10655,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C5" t="n">
         <v>5</v>
@@ -10668,7 +10668,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C6" t="n">
         <v>4</v>
@@ -10681,7 +10681,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C7" t="n">
         <v>5</v>

</xml_diff>